<commit_message>
added code UpperCase and VowelCOunt
</commit_message>
<xml_diff>
--- a/TestData/testdata.xlsx
+++ b/TestData/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Project\Testing_Project\interviewPractice2026\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A68228-29F8-4A04-98C6-E426A43FB73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D3AC1C-E6B4-4C40-8AF7-28199DD73517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Masum</t>
   </si>
@@ -34,6 +34,21 @@
   </si>
   <si>
     <t>Delhi</t>
+  </si>
+  <si>
+    <t>Patna</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Amnour</t>
+  </si>
+  <si>
+    <t>Saran</t>
   </si>
 </sst>
 </file>
@@ -351,27 +366,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>